<commit_message>
2018/10/31 1. "side to front" with top bottom black area. 2. clear middle area using 2/3 height white main spine.
</commit_message>
<xml_diff>
--- a/spine影像統計.xlsx
+++ b/spine影像統計.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>總數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,10 @@
   </si>
   <si>
     <t>65、64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消失：24、39、68、73、92、102</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -402,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -487,6 +491,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2018/12/10 1. fill the missing middle part with average box size rectangle
</commit_message>
<xml_diff>
--- a/spine影像統計.xlsx
+++ b/spine影像統計.xlsx
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AD30" sqref="AC1:AD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2019/01/03 1.save original size saggital spine
</commit_message>
<xml_diff>
--- a/spine影像統計.xlsx
+++ b/spine影像統計.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
   <si>
     <t>總數</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -400,11 +400,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>40、60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沒標記、補完怪</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>多截一段、多上面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>2、3、5、6、9、11、13、15、19、21、27、35、38、42、49、53、56、61、64、65、72、74、75、77、78、79、81、82、89、90、91、93、94、</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>40、60</t>
+    <t>備註20181221 補最下面0.9h格的位置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、3、5、6、9、11、13、15、19、21、27、35、38、40、42、49、53、56、61、64、65、72、74、75、77、78、79、81、82、89、90、91、93、94、</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>60、</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -778,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH60"/>
+  <dimension ref="A1:AL60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AD22" sqref="AD22"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -790,9 +810,10 @@
     <col min="25" max="25" width="31.625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="33.875" customWidth="1"/>
     <col min="33" max="33" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="37.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -832,8 +853,12 @@
         <v>93</v>
       </c>
       <c r="AH1" s="1"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL1" s="1"/>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -860,7 +885,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -895,8 +920,11 @@
       <c r="AG3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -929,10 +957,16 @@
         <v>46</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>9</v>
       </c>
@@ -963,8 +997,14 @@
       <c r="AH5" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="O6" t="s">
         <v>22</v>
       </c>
@@ -987,10 +1027,16 @@
         <v>95</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="O7" t="s">
         <v>21</v>
       </c>
@@ -1011,8 +1057,10 @@
       </c>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1042,8 +1090,10 @@
       </c>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1</v>
       </c>
@@ -1074,8 +1124,14 @@
       <c r="AH9" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1098,8 +1154,14 @@
       <c r="AH10" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1128,7 +1190,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>12</v>
       </c>
@@ -1159,8 +1221,14 @@
       <c r="AH12" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>14</v>
       </c>
@@ -1179,8 +1247,14 @@
       <c r="AH13" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>16</v>
       </c>
@@ -1204,8 +1278,10 @@
       </c>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>20</v>
       </c>
@@ -1233,8 +1309,14 @@
       <c r="AH15" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AK15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL15" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>22</v>
       </c>
@@ -1258,8 +1340,14 @@
       <c r="AH16" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>25</v>
       </c>
@@ -1278,13 +1366,19 @@
         <v>90</v>
       </c>
       <c r="AG17" s="1" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="AH17" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>34</v>
       </c>
@@ -1308,8 +1402,10 @@
       </c>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
-    </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+    </row>
+    <row r="19" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>35</v>
       </c>
@@ -1330,8 +1426,10 @@
       </c>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
-    </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+    </row>
+    <row r="20" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>36</v>
       </c>
@@ -1355,8 +1453,14 @@
       <c r="AH20" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>39</v>
       </c>
@@ -1375,13 +1479,19 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
       <c r="AG21" s="1" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="AH21" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>41</v>
       </c>
@@ -1405,8 +1515,14 @@
       <c r="AH22" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>44</v>
       </c>
@@ -1427,8 +1543,10 @@
       </c>
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
-    </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK23" s="1"/>
+      <c r="AL23" s="1"/>
+    </row>
+    <row r="24" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>45</v>
       </c>
@@ -1456,8 +1574,14 @@
       <c r="AH24" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL24" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>47</v>
       </c>
@@ -1481,8 +1605,14 @@
       <c r="AH25" s="1">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL25" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>51</v>
       </c>
@@ -1506,8 +1636,14 @@
       <c r="AH26" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL26" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>52</v>
       </c>
@@ -1532,8 +1668,14 @@
       <c r="AH27" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL27" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>57</v>
       </c>
@@ -1553,7 +1695,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>58</v>
       </c>
@@ -1573,7 +1715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>62</v>
       </c>
@@ -1581,7 +1723,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>63</v>
       </c>
@@ -1589,7 +1731,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>73</v>
       </c>

</xml_diff>